<commit_message>
updated search in faq
</commit_message>
<xml_diff>
--- a/faq/faq.xlsx
+++ b/faq/faq.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Что такое перепланировка? Чем перепланировка отличается от переустройства?</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Требуется ли согласование на изменение переплета окна (оконное заполнение, рисунок, конфигурация рам)?</t>
-  </si>
-  <si>
-    <t>Что-то</t>
   </si>
   <si>
     <t>В соответствии со ст. 25 Жилищного кодекса Российской Федерации перепланировкой помещения в многоквартирном доме является изменение его конфигурации, требующее внесения изменения в технический паспорт помещения в многоквартирном доме.
@@ -357,9 +354,6 @@
   </si>
   <si>
     <t>Данные мероприятия не относятся к работам по переустройству и перепланировке, и не требуют согласования с Мосжилинспекцией.</t>
-  </si>
-  <si>
-    <t>кто-то</t>
   </si>
 </sst>
 </file>
@@ -701,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -726,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -734,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -742,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -750,7 +744,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -758,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -766,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -774,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -782,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -790,7 +784,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -798,7 +792,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -806,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -814,7 +808,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -822,7 +816,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -830,7 +824,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -838,7 +832,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -846,7 +840,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -854,7 +848,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -862,7 +856,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -870,7 +864,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -878,7 +872,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -886,7 +880,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -894,7 +888,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -902,7 +896,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -910,7 +904,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -918,7 +912,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -926,7 +920,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -934,7 +928,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -942,7 +936,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -950,7 +944,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -958,7 +952,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -966,7 +960,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -974,7 +968,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -982,7 +976,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -990,7 +984,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -998,15 +992,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>